<commit_message>
QC script modified and input files added
</commit_message>
<xml_diff>
--- a/data/_input/data_export_WIISE_V_COV_UPTAKE_GENDER_LAST_MONTH_LONG.xlsx
+++ b/data/_input/data_export_WIISE_V_COV_UPTAKE_GENDER_LAST_MONTH_LONG.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="331">
   <si>
     <t>ISO_3_CODE</t>
   </si>
@@ -377,7 +377,10 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>This category includes the "Other" and "Not reported" categories.</t>
+    <t>Ongoing data quality assurance activities can result in unexpected decreases of cumulative numbers from a report to another, as historical data correction and update is not available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This category includes the "Other" and "Not reported" categories. </t>
   </si>
   <si>
     <t>CHL</t>
@@ -743,241 +746,244 @@
     <t>New Zealand</t>
   </si>
   <si>
+    <t>Unknown gender includes missing information, few records have been updated in the last month and now classified under Male/Female</t>
+  </si>
+  <si>
+    <t>OMN</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>PAK</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>PNG</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>PRY</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>occupied Palestinian territory, including east Jerusalem</t>
+  </si>
+  <si>
+    <t>PYF</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>QAT</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>RWA</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>SAU</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data here are taken from our electronic system (tracking system),as its not available on the (paper based/registry books),therefore you will find discrepancies regarding the numbers from the tables above , due to having more data from the paper based </t>
+  </si>
+  <si>
+    <t>SEN</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>SLE</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>SLV</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>HUBO UN ERRO INVOLUNTARIO EN EL INFORME DEL MES ANTERIOR</t>
+  </si>
+  <si>
+    <t>SMR</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>2021-03</t>
+  </si>
+  <si>
+    <t>SOM</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>STP</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>SWZ</t>
+  </si>
+  <si>
+    <t>Eswatini</t>
+  </si>
+  <si>
+    <t>SYR</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>THA</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccination uptake data coming from SEAR data collection tool</t>
+  </si>
+  <si>
+    <t>TLS</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>2022-01</t>
+  </si>
+  <si>
+    <t>01-January</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>2021-04</t>
+  </si>
+  <si>
+    <t>TZA</t>
+  </si>
+  <si>
+    <t>United Republic of Tanzania</t>
+  </si>
+  <si>
+    <t>No comment</t>
+  </si>
+  <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>UKR</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>URY</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>VCT</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>VEN</t>
+  </si>
+  <si>
+    <t>Venezuela (Bolivarian Republic of)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>VGB</t>
+  </si>
+  <si>
+    <t>British Virgin Islands</t>
+  </si>
+  <si>
+    <t>WSM</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>XKX</t>
+  </si>
+  <si>
+    <t>Kosovo (in accordance with UN Security Council resolution 1244 (1999))</t>
+  </si>
+  <si>
+    <t>UNICEF Programme</t>
+  </si>
+  <si>
     <t>2021-10</t>
   </si>
   <si>
     <t>10-October</t>
-  </si>
-  <si>
-    <t>OMN</t>
-  </si>
-  <si>
-    <t>Oman</t>
-  </si>
-  <si>
-    <t>PAK</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>PNG</t>
-  </si>
-  <si>
-    <t>Papua New Guinea</t>
-  </si>
-  <si>
-    <t>PRY</t>
-  </si>
-  <si>
-    <t>Paraguay</t>
-  </si>
-  <si>
-    <t>PSE</t>
-  </si>
-  <si>
-    <t>occupied Palestinian territory, including east Jerusalem</t>
-  </si>
-  <si>
-    <t>PYF</t>
-  </si>
-  <si>
-    <t>French Polynesia</t>
-  </si>
-  <si>
-    <t>QAT</t>
-  </si>
-  <si>
-    <t>Qatar</t>
-  </si>
-  <si>
-    <t>RWA</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
-  </si>
-  <si>
-    <t>SAU</t>
-  </si>
-  <si>
-    <t>Saudi Arabia</t>
-  </si>
-  <si>
-    <t>SDN</t>
-  </si>
-  <si>
-    <t>Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The data here are taken from our electronic system (tracking system),as its not available on the (paper based/registry books),therefore you will find discrepancies regarding the numbers from the tables above , due to having more data from the paper based </t>
-  </si>
-  <si>
-    <t>SEN</t>
-  </si>
-  <si>
-    <t>Senegal</t>
-  </si>
-  <si>
-    <t>SLE</t>
-  </si>
-  <si>
-    <t>Sierra Leone</t>
-  </si>
-  <si>
-    <t>SLV</t>
-  </si>
-  <si>
-    <t>El Salvador</t>
-  </si>
-  <si>
-    <t>HUBO UN ERRO INVOLUNTARIO EN EL INFORME DEL MES ANTERIOR</t>
-  </si>
-  <si>
-    <t>SMR</t>
-  </si>
-  <si>
-    <t>San Marino</t>
-  </si>
-  <si>
-    <t>2021-03</t>
-  </si>
-  <si>
-    <t>SOM</t>
-  </si>
-  <si>
-    <t>Somalia</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>South Sudan</t>
-  </si>
-  <si>
-    <t>STP</t>
-  </si>
-  <si>
-    <t>Sao Tome and Principe</t>
-  </si>
-  <si>
-    <t>SWZ</t>
-  </si>
-  <si>
-    <t>Eswatini</t>
-  </si>
-  <si>
-    <t>SYR</t>
-  </si>
-  <si>
-    <t>Syrian Arab Republic</t>
-  </si>
-  <si>
-    <t>TCD</t>
-  </si>
-  <si>
-    <t>Chad</t>
-  </si>
-  <si>
-    <t>THA</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
-    <t>COVID-19 vaccination uptake data coming from SEAR data collection tool</t>
-  </si>
-  <si>
-    <t>TLS</t>
-  </si>
-  <si>
-    <t>Timor-Leste</t>
-  </si>
-  <si>
-    <t>2022-01</t>
-  </si>
-  <si>
-    <t>01-January</t>
-  </si>
-  <si>
-    <t>TON</t>
-  </si>
-  <si>
-    <t>Tonga</t>
-  </si>
-  <si>
-    <t>2021-04</t>
-  </si>
-  <si>
-    <t>TZA</t>
-  </si>
-  <si>
-    <t>United Republic of Tanzania</t>
-  </si>
-  <si>
-    <t>No comment</t>
-  </si>
-  <si>
-    <t>UGA</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>UKR</t>
-  </si>
-  <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
-    <t>URY</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>United States of America</t>
-  </si>
-  <si>
-    <t>VCT</t>
-  </si>
-  <si>
-    <t>Saint Vincent and the Grenadines</t>
-  </si>
-  <si>
-    <t>VEN</t>
-  </si>
-  <si>
-    <t>Venezuela (Bolivarian Republic of)</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>VGB</t>
-  </si>
-  <si>
-    <t>British Virgin Islands</t>
-  </si>
-  <si>
-    <t>WSM</t>
-  </si>
-  <si>
-    <t>Samoa</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>XKX</t>
-  </si>
-  <si>
-    <t>Kosovo (in accordance with UN Security Council resolution 1244 (1999))</t>
-  </si>
-  <si>
-    <t>UNICEF Programme</t>
   </si>
   <si>
     <t>YEM</t>
@@ -3177,16 +3183,16 @@
         <v>38</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="L23" s="0">
         <v>2022</v>
       </c>
       <c r="M23" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="O23" s="0" t="s">
         <v>41</v>
@@ -3207,31 +3213,31 @@
         <v>84788982</v>
       </c>
       <c r="U23" s="0">
-        <v>63513692</v>
+        <v>63962318</v>
       </c>
       <c r="V23" s="0">
-        <v>55548456</v>
+        <v>57590671</v>
       </c>
       <c r="W23" s="0" t="s">
         <v>45</v>
       </c>
       <c r="X23" s="0">
-        <v>5302745</v>
+        <v>7061529</v>
       </c>
       <c r="Y23" s="0">
-        <v>7965236</v>
+        <v>6371647</v>
       </c>
       <c r="Z23" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AA23" s="0">
-        <v>21275290</v>
+        <v>20826664</v>
       </c>
       <c r="AB23" s="0">
-        <v>74.907954432098279</v>
+        <v>75.437063273150272</v>
       </c>
       <c r="AC23" s="0">
-        <v>65.513766871266355</v>
+        <v>67.922352222603635</v>
       </c>
       <c r="AD23" s="0" t="s">
         <v>45</v>
@@ -3269,16 +3275,16 @@
         <v>38</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="L24" s="0">
         <v>2022</v>
       </c>
       <c r="M24" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="O24" s="0" t="s">
         <v>41</v>
@@ -3299,31 +3305,31 @@
         <v>83096698</v>
       </c>
       <c r="U24" s="0">
-        <v>64160861</v>
+        <v>64606302</v>
       </c>
       <c r="V24" s="0">
-        <v>56810633</v>
+        <v>58834608</v>
       </c>
       <c r="W24" s="0" t="s">
         <v>45</v>
       </c>
       <c r="X24" s="0">
-        <v>4163676</v>
+        <v>5737784</v>
       </c>
       <c r="Y24" s="0">
-        <v>7350228</v>
+        <v>5771694</v>
       </c>
       <c r="Z24" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AA24" s="0">
-        <v>18935837</v>
+        <v>18490396</v>
       </c>
       <c r="AB24" s="0">
-        <v>77.212287063440243</v>
+        <v>77.74833844781655</v>
       </c>
       <c r="AC24" s="0">
-        <v>68.366895878341637</v>
+        <v>70.802582311995124</v>
       </c>
       <c r="AD24" s="0" t="s">
         <v>45</v>
@@ -3361,16 +3367,16 @@
         <v>38</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="L25" s="0">
         <v>2022</v>
       </c>
       <c r="M25" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="O25" s="0" t="s">
         <v>41</v>
@@ -5477,16 +5483,16 @@
         <v>38</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="L48" s="0">
         <v>2022</v>
       </c>
       <c r="M48" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N48" s="0" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="O48" s="0" t="s">
         <v>41</v>
@@ -5501,40 +5507,40 @@
         <v>44</v>
       </c>
       <c r="S48" s="0">
-        <v>19006183</v>
+        <v>19006265</v>
       </c>
       <c r="T48" s="0">
         <v>19060905</v>
       </c>
       <c r="U48" s="0">
-        <v>15856645</v>
+        <v>15904575</v>
       </c>
       <c r="V48" s="0">
-        <v>15061738</v>
+        <v>15240543</v>
       </c>
       <c r="W48" s="0" t="s">
         <v>45</v>
       </c>
       <c r="X48" s="0">
-        <v>8099057</v>
+        <v>8506330</v>
       </c>
       <c r="Y48" s="0">
-        <v>794907</v>
+        <v>664032</v>
       </c>
       <c r="Z48" s="0">
-        <v>3149538</v>
+        <v>3101690</v>
       </c>
       <c r="AA48" s="0">
-        <v>3204260</v>
+        <v>3156330</v>
       </c>
       <c r="AB48" s="0">
-        <v>83.1893606310928</v>
+        <v>83.440817736618484</v>
       </c>
       <c r="AC48" s="0">
-        <v>79.019007754353737</v>
+        <v>79.9570796874545</v>
       </c>
       <c r="AD48" s="0" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49">
@@ -5569,16 +5575,16 @@
         <v>38</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="L49" s="0">
         <v>2022</v>
       </c>
       <c r="M49" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N49" s="0" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="O49" s="0" t="s">
         <v>41</v>
@@ -5593,40 +5599,40 @@
         <v>47</v>
       </c>
       <c r="S49" s="0">
-        <v>19237853</v>
+        <v>19237944</v>
       </c>
       <c r="T49" s="0">
         <v>19327511</v>
       </c>
       <c r="U49" s="0">
-        <v>16458834</v>
+        <v>16505165</v>
       </c>
       <c r="V49" s="0">
-        <v>15756958</v>
+        <v>15925526</v>
       </c>
       <c r="W49" s="0" t="s">
         <v>45</v>
       </c>
       <c r="X49" s="0">
-        <v>9376654</v>
+        <v>9818933</v>
       </c>
       <c r="Y49" s="0">
-        <v>701876</v>
+        <v>579639</v>
       </c>
       <c r="Z49" s="0">
-        <v>2779019</v>
+        <v>2732779</v>
       </c>
       <c r="AA49" s="0">
-        <v>2868677</v>
+        <v>2822346</v>
       </c>
       <c r="AB49" s="0">
-        <v>85.157545635338138</v>
+        <v>85.3972609302874</v>
       </c>
       <c r="AC49" s="0">
-        <v>81.526058890873216</v>
+        <v>82.398224996483</v>
       </c>
       <c r="AD49" s="0" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50">
@@ -5661,16 +5667,16 @@
         <v>38</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="L50" s="0">
         <v>2022</v>
       </c>
       <c r="M50" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N50" s="0" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="O50" s="0" t="s">
         <v>41</v>
@@ -5691,19 +5697,19 @@
         <v>45</v>
       </c>
       <c r="U50" s="0">
-        <v>35002</v>
+        <v>34284</v>
       </c>
       <c r="V50" s="0">
-        <v>31344</v>
+        <v>30903</v>
       </c>
       <c r="W50" s="0" t="s">
         <v>45</v>
       </c>
       <c r="X50" s="0">
-        <v>16158</v>
+        <v>16780</v>
       </c>
       <c r="Y50" s="0">
-        <v>3658</v>
+        <v>3381</v>
       </c>
       <c r="Z50" s="0" t="s">
         <v>45</v>
@@ -5718,15 +5724,15 @@
         <v>45</v>
       </c>
       <c r="AD50" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>52</v>
@@ -5815,10 +5821,10 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>52</v>
@@ -5907,10 +5913,10 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>52</v>
@@ -5999,10 +6005,10 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>85</v>
@@ -6091,10 +6097,10 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>85</v>
@@ -6183,10 +6189,10 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>85</v>
@@ -6275,10 +6281,10 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>85</v>
@@ -6367,10 +6373,10 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>52</v>
@@ -6454,15 +6460,15 @@
         <v>41.001026864980346</v>
       </c>
       <c r="AD58" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>52</v>
@@ -6546,15 +6552,15 @@
         <v>44.4901283805456</v>
       </c>
       <c r="AD59" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>52</v>
@@ -6638,15 +6644,15 @@
         <v>45</v>
       </c>
       <c r="AD60" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>85</v>
@@ -6735,10 +6741,10 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>85</v>
@@ -6827,10 +6833,10 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>85</v>
@@ -6919,10 +6925,10 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>85</v>
@@ -7011,10 +7017,10 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>52</v>
@@ -7103,10 +7109,10 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>52</v>
@@ -7195,10 +7201,10 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>52</v>
@@ -7282,15 +7288,15 @@
         <v>45</v>
       </c>
       <c r="AD67" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>52</v>
@@ -7374,15 +7380,15 @@
         <v>45</v>
       </c>
       <c r="AD68" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>52</v>
@@ -7466,15 +7472,15 @@
         <v>45</v>
       </c>
       <c r="AD69" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>52</v>
@@ -7558,15 +7564,15 @@
         <v>45</v>
       </c>
       <c r="AD70" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>52</v>
@@ -7655,10 +7661,10 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>52</v>
@@ -7747,10 +7753,10 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>52</v>
@@ -7839,10 +7845,10 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>73</v>
@@ -7931,10 +7937,10 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>73</v>
@@ -8023,10 +8029,10 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>73</v>
@@ -8115,10 +8121,10 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>85</v>
@@ -8202,15 +8208,15 @@
         <v>18.438605766097918</v>
       </c>
       <c r="AD77" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>85</v>
@@ -8294,15 +8300,15 @@
         <v>16.34118427708469</v>
       </c>
       <c r="AD78" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>85</v>
@@ -8386,15 +8392,15 @@
         <v>45</v>
       </c>
       <c r="AD79" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>85</v>
@@ -8483,10 +8489,10 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>85</v>
@@ -8575,10 +8581,10 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>85</v>
@@ -8667,10 +8673,10 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>85</v>
@@ -8759,10 +8765,10 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>85</v>
@@ -8851,10 +8857,10 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>85</v>
@@ -8943,10 +8949,10 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>85</v>
@@ -9035,10 +9041,10 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>85</v>
@@ -9127,10 +9133,10 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>85</v>
@@ -9219,10 +9225,10 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>85</v>
@@ -9311,10 +9317,10 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>85</v>
@@ -9403,10 +9409,10 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>85</v>
@@ -9495,10 +9501,10 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>52</v>
@@ -9525,7 +9531,7 @@
         <v>38</v>
       </c>
       <c r="K92" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L92" s="0">
         <v>2021</v>
@@ -9534,7 +9540,7 @@
         <v>6</v>
       </c>
       <c r="N92" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O92" s="0" t="s">
         <v>41</v>
@@ -9587,10 +9593,10 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>52</v>
@@ -9617,7 +9623,7 @@
         <v>38</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L93" s="0">
         <v>2021</v>
@@ -9626,7 +9632,7 @@
         <v>6</v>
       </c>
       <c r="N93" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O93" s="0" t="s">
         <v>41</v>
@@ -9679,10 +9685,10 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>52</v>
@@ -9771,10 +9777,10 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>52</v>
@@ -9863,10 +9869,10 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>52</v>
@@ -9955,10 +9961,10 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>66</v>
@@ -9979,7 +9985,7 @@
         <v>69</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J97" s="0" t="s">
         <v>56</v>
@@ -10047,10 +10053,10 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>66</v>
@@ -10071,7 +10077,7 @@
         <v>69</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J98" s="0" t="s">
         <v>56</v>
@@ -10139,10 +10145,10 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>66</v>
@@ -10163,7 +10169,7 @@
         <v>69</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J99" s="0" t="s">
         <v>56</v>
@@ -10231,10 +10237,10 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>52</v>
@@ -10323,10 +10329,10 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>52</v>
@@ -10415,10 +10421,10 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>52</v>
@@ -10507,10 +10513,10 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C103" s="0" t="s">
         <v>95</v>
@@ -10599,10 +10605,10 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>95</v>
@@ -10691,10 +10697,10 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>95</v>
@@ -10783,10 +10789,10 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>95</v>
@@ -10870,15 +10876,15 @@
         <v>45</v>
       </c>
       <c r="AD106" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>95</v>
@@ -10962,15 +10968,15 @@
         <v>45</v>
       </c>
       <c r="AD107" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>95</v>
@@ -11059,10 +11065,10 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>73</v>
@@ -11146,15 +11152,15 @@
         <v>11.984424539593689</v>
       </c>
       <c r="AD109" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>73</v>
@@ -11243,16 +11249,16 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>32</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E111" s="0" t="s">
         <v>59</v>
@@ -11335,16 +11341,16 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>32</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E112" s="0" t="s">
         <v>59</v>
@@ -11427,16 +11433,16 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>32</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E113" s="0" t="s">
         <v>59</v>
@@ -11519,10 +11525,10 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>73</v>
@@ -11611,10 +11617,10 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>73</v>
@@ -11703,10 +11709,10 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>73</v>
@@ -11795,10 +11801,10 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>52</v>
@@ -11882,15 +11888,15 @@
         <v>25.583787785547287</v>
       </c>
       <c r="AD117" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>52</v>
@@ -11974,15 +11980,15 @@
         <v>45</v>
       </c>
       <c r="AD118" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>52</v>
@@ -12066,15 +12072,15 @@
         <v>20.422063775673912</v>
       </c>
       <c r="AD119" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>85</v>
@@ -12163,10 +12169,10 @@
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>85</v>
@@ -12255,10 +12261,10 @@
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C122" s="0" t="s">
         <v>73</v>
@@ -12285,7 +12291,7 @@
         <v>38</v>
       </c>
       <c r="K122" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L122" s="0">
         <v>2021</v>
@@ -12294,7 +12300,7 @@
         <v>7</v>
       </c>
       <c r="N122" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O122" s="0" t="s">
         <v>41</v>
@@ -12347,10 +12353,10 @@
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C123" s="0" t="s">
         <v>73</v>
@@ -12377,7 +12383,7 @@
         <v>38</v>
       </c>
       <c r="K123" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L123" s="0">
         <v>2021</v>
@@ -12386,7 +12392,7 @@
         <v>7</v>
       </c>
       <c r="N123" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O123" s="0" t="s">
         <v>41</v>
@@ -12439,10 +12445,10 @@
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>73</v>
@@ -12469,7 +12475,7 @@
         <v>38</v>
       </c>
       <c r="K124" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L124" s="0">
         <v>2021</v>
@@ -12478,7 +12484,7 @@
         <v>7</v>
       </c>
       <c r="N124" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O124" s="0" t="s">
         <v>41</v>
@@ -12531,10 +12537,10 @@
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C125" s="0" t="s">
         <v>66</v>
@@ -12623,10 +12629,10 @@
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C126" s="0" t="s">
         <v>66</v>
@@ -12715,10 +12721,10 @@
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C127" s="0" t="s">
         <v>66</v>
@@ -12745,7 +12751,7 @@
         <v>38</v>
       </c>
       <c r="K127" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L127" s="0">
         <v>2021</v>
@@ -12754,7 +12760,7 @@
         <v>8</v>
       </c>
       <c r="N127" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="O127" s="0" t="s">
         <v>41</v>
@@ -12807,10 +12813,10 @@
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>66</v>
@@ -12837,7 +12843,7 @@
         <v>38</v>
       </c>
       <c r="K128" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L128" s="0">
         <v>2021</v>
@@ -12846,7 +12852,7 @@
         <v>8</v>
       </c>
       <c r="N128" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="O128" s="0" t="s">
         <v>41</v>
@@ -12899,10 +12905,10 @@
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C129" s="0" t="s">
         <v>66</v>
@@ -12929,7 +12935,7 @@
         <v>38</v>
       </c>
       <c r="K129" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L129" s="0">
         <v>2021</v>
@@ -12938,7 +12944,7 @@
         <v>8</v>
       </c>
       <c r="N129" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="O129" s="0" t="s">
         <v>41</v>
@@ -12986,15 +12992,15 @@
         <v>26.91737288993609</v>
       </c>
       <c r="AD129" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C130" s="0" t="s">
         <v>85</v>
@@ -13083,10 +13089,10 @@
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C131" s="0" t="s">
         <v>85</v>
@@ -13175,10 +13181,10 @@
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>85</v>
@@ -13262,15 +13268,15 @@
         <v>45</v>
       </c>
       <c r="AD132" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C133" s="0" t="s">
         <v>73</v>
@@ -13297,7 +13303,7 @@
         <v>38</v>
       </c>
       <c r="K133" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L133" s="0">
         <v>2021</v>
@@ -13306,7 +13312,7 @@
         <v>12</v>
       </c>
       <c r="N133" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O133" s="0" t="s">
         <v>41</v>
@@ -13359,10 +13365,10 @@
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C134" s="0" t="s">
         <v>73</v>
@@ -13389,7 +13395,7 @@
         <v>38</v>
       </c>
       <c r="K134" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L134" s="0">
         <v>2021</v>
@@ -13398,7 +13404,7 @@
         <v>12</v>
       </c>
       <c r="N134" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O134" s="0" t="s">
         <v>41</v>
@@ -13451,10 +13457,10 @@
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>73</v>
@@ -13481,7 +13487,7 @@
         <v>38</v>
       </c>
       <c r="K135" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L135" s="0">
         <v>2021</v>
@@ -13490,7 +13496,7 @@
         <v>12</v>
       </c>
       <c r="N135" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O135" s="0" t="s">
         <v>41</v>
@@ -13543,10 +13549,10 @@
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C136" s="0" t="s">
         <v>66</v>
@@ -13567,7 +13573,7 @@
         <v>69</v>
       </c>
       <c r="I136" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J136" s="0" t="s">
         <v>56</v>
@@ -13635,10 +13641,10 @@
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C137" s="0" t="s">
         <v>66</v>
@@ -13659,7 +13665,7 @@
         <v>69</v>
       </c>
       <c r="I137" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J137" s="0" t="s">
         <v>56</v>
@@ -13727,10 +13733,10 @@
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C138" s="0" t="s">
         <v>66</v>
@@ -13751,7 +13757,7 @@
         <v>69</v>
       </c>
       <c r="I138" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J138" s="0" t="s">
         <v>56</v>
@@ -13819,10 +13825,10 @@
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C139" s="0" t="s">
         <v>73</v>
@@ -13911,10 +13917,10 @@
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C140" s="0" t="s">
         <v>73</v>
@@ -14003,10 +14009,10 @@
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C141" s="0" t="s">
         <v>73</v>
@@ -14095,10 +14101,10 @@
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C142" s="0" t="s">
         <v>85</v>
@@ -14187,10 +14193,10 @@
     </row>
     <row r="143">
       <c r="A143" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C143" s="0" t="s">
         <v>85</v>
@@ -14279,10 +14285,10 @@
     </row>
     <row r="144">
       <c r="A144" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C144" s="0" t="s">
         <v>85</v>
@@ -14371,10 +14377,10 @@
     </row>
     <row r="145">
       <c r="A145" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C145" s="0" t="s">
         <v>52</v>
@@ -14463,10 +14469,10 @@
     </row>
     <row r="146">
       <c r="A146" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C146" s="0" t="s">
         <v>52</v>
@@ -14555,10 +14561,10 @@
     </row>
     <row r="147">
       <c r="A147" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C147" s="0" t="s">
         <v>52</v>
@@ -14647,10 +14653,10 @@
     </row>
     <row r="148">
       <c r="A148" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C148" s="0" t="s">
         <v>85</v>
@@ -14739,10 +14745,10 @@
     </row>
     <row r="149">
       <c r="A149" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C149" s="0" t="s">
         <v>85</v>
@@ -14831,10 +14837,10 @@
     </row>
     <row r="150">
       <c r="A150" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C150" s="0" t="s">
         <v>66</v>
@@ -14918,15 +14924,15 @@
         <v>45</v>
       </c>
       <c r="AD150" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C151" s="0" t="s">
         <v>66</v>
@@ -15010,15 +15016,15 @@
         <v>45</v>
       </c>
       <c r="AD151" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C152" s="0" t="s">
         <v>85</v>
@@ -15107,10 +15113,10 @@
     </row>
     <row r="153">
       <c r="A153" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C153" s="0" t="s">
         <v>85</v>
@@ -15199,10 +15205,10 @@
     </row>
     <row r="154">
       <c r="A154" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C154" s="0" t="s">
         <v>85</v>
@@ -15291,10 +15297,10 @@
     </row>
     <row r="155">
       <c r="A155" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C155" s="0" t="s">
         <v>85</v>
@@ -15383,10 +15389,10 @@
     </row>
     <row r="156">
       <c r="A156" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C156" s="0" t="s">
         <v>66</v>
@@ -15413,7 +15419,7 @@
         <v>38</v>
       </c>
       <c r="K156" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L156" s="0">
         <v>2021</v>
@@ -15422,7 +15428,7 @@
         <v>12</v>
       </c>
       <c r="N156" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O156" s="0" t="s">
         <v>41</v>
@@ -15475,10 +15481,10 @@
     </row>
     <row r="157">
       <c r="A157" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C157" s="0" t="s">
         <v>66</v>
@@ -15505,7 +15511,7 @@
         <v>38</v>
       </c>
       <c r="K157" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L157" s="0">
         <v>2021</v>
@@ -15514,7 +15520,7 @@
         <v>12</v>
       </c>
       <c r="N157" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O157" s="0" t="s">
         <v>41</v>
@@ -15567,10 +15573,10 @@
     </row>
     <row r="158">
       <c r="A158" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C158" s="0" t="s">
         <v>66</v>
@@ -15597,7 +15603,7 @@
         <v>38</v>
       </c>
       <c r="K158" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L158" s="0">
         <v>2021</v>
@@ -15606,7 +15612,7 @@
         <v>12</v>
       </c>
       <c r="N158" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O158" s="0" t="s">
         <v>41</v>
@@ -15659,10 +15665,10 @@
     </row>
     <row r="159">
       <c r="A159" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C159" s="0" t="s">
         <v>85</v>
@@ -15751,10 +15757,10 @@
     </row>
     <row r="160">
       <c r="A160" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C160" s="0" t="s">
         <v>85</v>
@@ -15843,10 +15849,10 @@
     </row>
     <row r="161">
       <c r="A161" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C161" s="0" t="s">
         <v>85</v>
@@ -15935,10 +15941,10 @@
     </row>
     <row r="162">
       <c r="A162" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C162" s="0" t="s">
         <v>85</v>
@@ -16027,10 +16033,10 @@
     </row>
     <row r="163">
       <c r="A163" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C163" s="0" t="s">
         <v>52</v>
@@ -16057,7 +16063,7 @@
         <v>38</v>
       </c>
       <c r="K163" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L163" s="0">
         <v>2021</v>
@@ -16066,7 +16072,7 @@
         <v>12</v>
       </c>
       <c r="N163" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O163" s="0" t="s">
         <v>41</v>
@@ -16114,15 +16120,15 @@
         <v>39.860314942274712</v>
       </c>
       <c r="AD163" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C164" s="0" t="s">
         <v>52</v>
@@ -16149,7 +16155,7 @@
         <v>38</v>
       </c>
       <c r="K164" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L164" s="0">
         <v>2021</v>
@@ -16158,7 +16164,7 @@
         <v>12</v>
       </c>
       <c r="N164" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O164" s="0" t="s">
         <v>41</v>
@@ -16206,15 +16212,15 @@
         <v>47.341018594189158</v>
       </c>
       <c r="AD164" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C165" s="0" t="s">
         <v>52</v>
@@ -16241,7 +16247,7 @@
         <v>38</v>
       </c>
       <c r="K165" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L165" s="0">
         <v>2021</v>
@@ -16250,7 +16256,7 @@
         <v>12</v>
       </c>
       <c r="N165" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O165" s="0" t="s">
         <v>41</v>
@@ -16303,10 +16309,10 @@
     </row>
     <row r="166">
       <c r="A166" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C166" s="0" t="s">
         <v>73</v>
@@ -16390,15 +16396,15 @@
         <v>22.039305281681926</v>
       </c>
       <c r="AD166" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C167" s="0" t="s">
         <v>73</v>
@@ -16482,15 +16488,15 @@
         <v>14.864262560777957</v>
       </c>
       <c r="AD167" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C168" s="0" t="s">
         <v>66</v>
@@ -16517,16 +16523,16 @@
         <v>38</v>
       </c>
       <c r="K168" s="0" t="s">
-        <v>243</v>
+        <v>39</v>
       </c>
       <c r="L168" s="0">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="M168" s="0">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N168" s="0" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="O168" s="0" t="s">
         <v>41</v>
@@ -16541,37 +16547,37 @@
         <v>44</v>
       </c>
       <c r="S168" s="0">
-        <v>2042144</v>
+        <v>2286894</v>
       </c>
       <c r="T168" s="0">
-        <v>2388860</v>
+        <v>2407196</v>
       </c>
       <c r="U168" s="0">
-        <v>1815478</v>
+        <v>2131538</v>
       </c>
       <c r="V168" s="0">
-        <v>1529752</v>
+        <v>2029240</v>
       </c>
       <c r="W168" s="0" t="s">
         <v>45</v>
       </c>
       <c r="X168" s="0">
-        <v>5</v>
+        <v>1251594</v>
       </c>
       <c r="Y168" s="0">
-        <v>285726</v>
+        <v>102298</v>
       </c>
       <c r="Z168" s="0">
-        <v>226666</v>
+        <v>155356</v>
       </c>
       <c r="AA168" s="0">
-        <v>573382</v>
+        <v>275658</v>
       </c>
       <c r="AB168" s="0">
-        <v>75.9976725299934</v>
+        <v>88.5485851588321</v>
       </c>
       <c r="AC168" s="0">
-        <v>64.0369046323351</v>
+        <v>84.298910433550077</v>
       </c>
       <c r="AD168" s="0" t="s">
         <v>45</v>
@@ -16579,10 +16585,10 @@
     </row>
     <row r="169">
       <c r="A169" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C169" s="0" t="s">
         <v>66</v>
@@ -16609,16 +16615,16 @@
         <v>38</v>
       </c>
       <c r="K169" s="0" t="s">
-        <v>243</v>
+        <v>39</v>
       </c>
       <c r="L169" s="0">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="M169" s="0">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N169" s="0" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="O169" s="0" t="s">
         <v>41</v>
@@ -16633,37 +16639,37 @@
         <v>47</v>
       </c>
       <c r="S169" s="0">
-        <v>2163310</v>
+        <v>2396709</v>
       </c>
       <c r="T169" s="0">
-        <v>2471782</v>
+        <v>2491005</v>
       </c>
       <c r="U169" s="0">
-        <v>1892008</v>
+        <v>2176205</v>
       </c>
       <c r="V169" s="0">
-        <v>1633061</v>
+        <v>2084087</v>
       </c>
       <c r="W169" s="0" t="s">
         <v>45</v>
       </c>
       <c r="X169" s="0">
-        <v>9</v>
+        <v>1410518</v>
       </c>
       <c r="Y169" s="0">
-        <v>258947</v>
+        <v>92118</v>
       </c>
       <c r="Z169" s="0">
-        <v>271302</v>
+        <v>220504</v>
       </c>
       <c r="AA169" s="0">
-        <v>579774</v>
+        <v>314800</v>
       </c>
       <c r="AB169" s="0">
-        <v>76.5442907181944</v>
+        <v>87.3625303843228</v>
       </c>
       <c r="AC169" s="0">
-        <v>66.068164587330116</v>
+        <v>83.66450488858915</v>
       </c>
       <c r="AD169" s="0" t="s">
         <v>45</v>
@@ -16671,10 +16677,10 @@
     </row>
     <row r="170">
       <c r="A170" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C170" s="0" t="s">
         <v>66</v>
@@ -16701,16 +16707,16 @@
         <v>38</v>
       </c>
       <c r="K170" s="0" t="s">
-        <v>243</v>
+        <v>39</v>
       </c>
       <c r="L170" s="0">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="M170" s="0">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N170" s="0" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="O170" s="0" t="s">
         <v>41</v>
@@ -16725,28 +16731,28 @@
         <v>49</v>
       </c>
       <c r="S170" s="0">
-        <v>1603</v>
+        <v>1748</v>
       </c>
       <c r="T170" s="0" t="s">
         <v>45</v>
       </c>
       <c r="U170" s="0">
-        <v>5442</v>
+        <v>5336</v>
       </c>
       <c r="V170" s="0">
-        <v>4655</v>
+        <v>5169</v>
       </c>
       <c r="W170" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="X170" s="0" t="s">
-        <v>45</v>
+      <c r="X170" s="0">
+        <v>2861</v>
       </c>
       <c r="Y170" s="0">
-        <v>787</v>
+        <v>167</v>
       </c>
       <c r="Z170" s="0">
-        <v>-3839</v>
+        <v>-3588</v>
       </c>
       <c r="AA170" s="0" t="s">
         <v>45</v>
@@ -16758,7 +16764,7 @@
         <v>45</v>
       </c>
       <c r="AD170" s="0" t="s">
-        <v>45</v>
+        <v>244</v>
       </c>
     </row>
     <row r="171">
@@ -16772,7 +16778,7 @@
         <v>32</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E171" s="0" t="s">
         <v>59</v>
@@ -16793,7 +16799,7 @@
         <v>38</v>
       </c>
       <c r="K171" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L171" s="0">
         <v>2021</v>
@@ -16802,7 +16808,7 @@
         <v>12</v>
       </c>
       <c r="N171" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O171" s="0" t="s">
         <v>41</v>
@@ -16864,7 +16870,7 @@
         <v>32</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E172" s="0" t="s">
         <v>59</v>
@@ -16885,7 +16891,7 @@
         <v>38</v>
       </c>
       <c r="K172" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L172" s="0">
         <v>2021</v>
@@ -16894,7 +16900,7 @@
         <v>12</v>
       </c>
       <c r="N172" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O172" s="0" t="s">
         <v>41</v>
@@ -16956,7 +16962,7 @@
         <v>32</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E173" s="0" t="s">
         <v>59</v>
@@ -16977,7 +16983,7 @@
         <v>38</v>
       </c>
       <c r="K173" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L173" s="0">
         <v>2021</v>
@@ -16986,7 +16992,7 @@
         <v>12</v>
       </c>
       <c r="N173" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O173" s="0" t="s">
         <v>41</v>
@@ -17876,7 +17882,7 @@
         <v>32</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E183" s="0" t="s">
         <v>34</v>
@@ -17968,7 +17974,7 @@
         <v>32</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E184" s="0" t="s">
         <v>34</v>
@@ -18060,7 +18066,7 @@
         <v>32</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E185" s="0" t="s">
         <v>34</v>
@@ -18428,7 +18434,7 @@
         <v>32</v>
       </c>
       <c r="D189" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E189" s="0" t="s">
         <v>59</v>
@@ -18520,7 +18526,7 @@
         <v>32</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E190" s="0" t="s">
         <v>59</v>
@@ -18612,7 +18618,7 @@
         <v>32</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E191" s="0" t="s">
         <v>59</v>
@@ -18888,7 +18894,7 @@
         <v>32</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E194" s="0" t="s">
         <v>59</v>
@@ -18980,7 +18986,7 @@
         <v>32</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E195" s="0" t="s">
         <v>59</v>
@@ -19072,7 +19078,7 @@
         <v>32</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E196" s="0" t="s">
         <v>59</v>
@@ -19164,7 +19170,7 @@
         <v>32</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E197" s="0" t="s">
         <v>34</v>
@@ -19256,7 +19262,7 @@
         <v>32</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E198" s="0" t="s">
         <v>34</v>
@@ -19348,7 +19354,7 @@
         <v>32</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E199" s="0" t="s">
         <v>34</v>
@@ -20289,7 +20295,7 @@
         <v>38</v>
       </c>
       <c r="K209" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L209" s="0">
         <v>2021</v>
@@ -20298,7 +20304,7 @@
         <v>12</v>
       </c>
       <c r="N209" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O209" s="0" t="s">
         <v>41</v>
@@ -20381,7 +20387,7 @@
         <v>38</v>
       </c>
       <c r="K210" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L210" s="0">
         <v>2021</v>
@@ -20390,7 +20396,7 @@
         <v>12</v>
       </c>
       <c r="N210" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O210" s="0" t="s">
         <v>41</v>
@@ -20473,7 +20479,7 @@
         <v>38</v>
       </c>
       <c r="K211" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L211" s="0">
         <v>2021</v>
@@ -20482,7 +20488,7 @@
         <v>12</v>
       </c>
       <c r="N211" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O211" s="0" t="s">
         <v>41</v>
@@ -21188,7 +21194,7 @@
         <v>32</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E219" s="0" t="s">
         <v>34</v>
@@ -21280,7 +21286,7 @@
         <v>32</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E220" s="0" t="s">
         <v>34</v>
@@ -21372,7 +21378,7 @@
         <v>32</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E221" s="0" t="s">
         <v>34</v>
@@ -21669,7 +21675,7 @@
         <v>38</v>
       </c>
       <c r="K224" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L224" s="0">
         <v>2021</v>
@@ -21678,7 +21684,7 @@
         <v>6</v>
       </c>
       <c r="N224" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O224" s="0" t="s">
         <v>95</v>
@@ -21761,7 +21767,7 @@
         <v>38</v>
       </c>
       <c r="K225" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L225" s="0">
         <v>2021</v>
@@ -21770,7 +21776,7 @@
         <v>6</v>
       </c>
       <c r="N225" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O225" s="0" t="s">
         <v>95</v>
@@ -23601,7 +23607,7 @@
         <v>38</v>
       </c>
       <c r="K245" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L245" s="0">
         <v>2021</v>
@@ -23610,7 +23616,7 @@
         <v>7</v>
       </c>
       <c r="N245" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O245" s="0" t="s">
         <v>41</v>
@@ -23693,7 +23699,7 @@
         <v>38</v>
       </c>
       <c r="K246" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L246" s="0">
         <v>2021</v>
@@ -23702,7 +23708,7 @@
         <v>7</v>
       </c>
       <c r="N246" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O246" s="0" t="s">
         <v>41</v>
@@ -23785,7 +23791,7 @@
         <v>38</v>
       </c>
       <c r="K247" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L247" s="0">
         <v>2021</v>
@@ -23794,7 +23800,7 @@
         <v>7</v>
       </c>
       <c r="N247" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O247" s="0" t="s">
         <v>41</v>
@@ -24337,7 +24343,7 @@
         <v>38</v>
       </c>
       <c r="K253" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L253" s="0">
         <v>2021</v>
@@ -24346,7 +24352,7 @@
         <v>7</v>
       </c>
       <c r="N253" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O253" s="0" t="s">
         <v>41</v>
@@ -24429,7 +24435,7 @@
         <v>38</v>
       </c>
       <c r="K254" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L254" s="0">
         <v>2021</v>
@@ -24438,7 +24444,7 @@
         <v>7</v>
       </c>
       <c r="N254" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O254" s="0" t="s">
         <v>41</v>
@@ -24521,7 +24527,7 @@
         <v>38</v>
       </c>
       <c r="K255" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L255" s="0">
         <v>2021</v>
@@ -24530,7 +24536,7 @@
         <v>7</v>
       </c>
       <c r="N255" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O255" s="0" t="s">
         <v>41</v>
@@ -24613,7 +24619,7 @@
         <v>56</v>
       </c>
       <c r="K256" s="0" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="L256" s="0">
         <v>2021</v>
@@ -24622,7 +24628,7 @@
         <v>10</v>
       </c>
       <c r="N256" s="0" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="O256" s="0" t="s">
         <v>41</v>
@@ -24705,7 +24711,7 @@
         <v>56</v>
       </c>
       <c r="K257" s="0" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="L257" s="0">
         <v>2021</v>
@@ -24714,7 +24720,7 @@
         <v>10</v>
       </c>
       <c r="N257" s="0" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="O257" s="0" t="s">
         <v>41</v>
@@ -24797,7 +24803,7 @@
         <v>56</v>
       </c>
       <c r="K258" s="0" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="L258" s="0">
         <v>2021</v>
@@ -24806,7 +24812,7 @@
         <v>10</v>
       </c>
       <c r="N258" s="0" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="O258" s="0" t="s">
         <v>41</v>
@@ -24859,16 +24865,16 @@
     </row>
     <row r="259">
       <c r="A259" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B259" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C259" s="0" t="s">
         <v>32</v>
       </c>
       <c r="D259" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E259" s="0" t="s">
         <v>34</v>
@@ -24951,16 +24957,16 @@
     </row>
     <row r="260">
       <c r="A260" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B260" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C260" s="0" t="s">
         <v>32</v>
       </c>
       <c r="D260" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E260" s="0" t="s">
         <v>34</v>
@@ -25043,16 +25049,16 @@
     </row>
     <row r="261">
       <c r="A261" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C261" s="0" t="s">
         <v>32</v>
       </c>
       <c r="D261" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E261" s="0" t="s">
         <v>34</v>
@@ -25135,10 +25141,10 @@
     </row>
     <row r="262">
       <c r="A262" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B262" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C262" s="0" t="s">
         <v>85</v>
@@ -25227,10 +25233,10 @@
     </row>
     <row r="263">
       <c r="A263" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B263" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C263" s="0" t="s">
         <v>85</v>
@@ -25319,10 +25325,10 @@
     </row>
     <row r="264">
       <c r="A264" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B264" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C264" s="0" t="s">
         <v>85</v>
@@ -25406,15 +25412,15 @@
         <v>9.8831565314214043</v>
       </c>
       <c r="AD264" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B265" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C265" s="0" t="s">
         <v>85</v>
@@ -25498,15 +25504,15 @@
         <v>10.593388626033684</v>
       </c>
       <c r="AD265" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B266" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C266" s="0" t="s">
         <v>85</v>
@@ -25590,7 +25596,7 @@
         <v>45</v>
       </c>
       <c r="AD266" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -25599,228 +25605,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="504bd14f85abc770ed43885d52246388">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="823b5556cd3b486fc41cc4ce5ea1e5e3" ns2:_="" ns3:_="">
-    <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
-    <xsd:import namespace="62ca1376-8bea-4949-825e-fec085c3924e"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b370a6fa-a798-42e0-969d-19c284d8683f" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="62ca1376-8bea-4949-825e-fec085c3924e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501D815B-7972-4BAE-9651-903AC0B39C67}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1AE2C42-3208-4606-BE41-5DE45A339DE6}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5ABC3EC-9306-4510-B793-B28A9FF50CF8}"/>
 </file>
</xml_diff>